<commit_message>
finished state data pcp upload
Finished uploading state pcp data. Finalized state code. Currently clipping triangle data code based on state code run. Will remove once we know which version we will hand over.
</commit_message>
<xml_diff>
--- a/deploy/nc-water-supply/data_state/pcp/ncsu_api_locations.xlsx
+++ b/deploy/nc-water-supply/data_state/pcp/ncsu_api_locations.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2713" uniqueCount="914">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2801" uniqueCount="914">
   <si>
     <t>B Everett Jordan Dam</t>
   </si>
@@ -2774,7 +2774,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2786,6 +2786,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2823,7 +2830,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2832,6 +2839,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6969,8 +6977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="C154" sqref="C154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9332,6 +9340,9 @@
       <c r="B67">
         <v>314996</v>
       </c>
+      <c r="C67" s="8" t="s">
+        <v>406</v>
+      </c>
       <c r="D67" t="s">
         <v>1</v>
       </c>
@@ -9364,6 +9375,9 @@
       <c r="B68">
         <v>315340</v>
       </c>
+      <c r="C68" t="s">
+        <v>406</v>
+      </c>
       <c r="D68" t="s">
         <v>1</v>
       </c>
@@ -9399,6 +9413,9 @@
       <c r="B69">
         <v>315838</v>
       </c>
+      <c r="C69" t="s">
+        <v>406</v>
+      </c>
       <c r="D69" t="s">
         <v>1</v>
       </c>
@@ -9434,6 +9451,9 @@
       <c r="B70">
         <v>315913</v>
       </c>
+      <c r="C70" t="s">
+        <v>406</v>
+      </c>
       <c r="D70" t="s">
         <v>1</v>
       </c>
@@ -9469,6 +9489,9 @@
       <c r="B71">
         <v>316380</v>
       </c>
+      <c r="C71" t="s">
+        <v>406</v>
+      </c>
       <c r="D71" t="s">
         <v>1</v>
       </c>
@@ -9501,6 +9524,9 @@
       <c r="B72">
         <v>317229</v>
       </c>
+      <c r="C72" t="s">
+        <v>406</v>
+      </c>
       <c r="D72" t="s">
         <v>1</v>
       </c>
@@ -9533,6 +9559,9 @@
       <c r="B73">
         <v>317845</v>
       </c>
+      <c r="C73" t="s">
+        <v>406</v>
+      </c>
       <c r="D73" t="s">
         <v>1</v>
       </c>
@@ -9568,6 +9597,9 @@
       <c r="B74">
         <v>318519</v>
       </c>
+      <c r="C74" t="s">
+        <v>406</v>
+      </c>
       <c r="D74" t="s">
         <v>1</v>
       </c>
@@ -9600,6 +9632,9 @@
       <c r="B75">
         <v>318744</v>
       </c>
+      <c r="C75" t="s">
+        <v>406</v>
+      </c>
       <c r="D75" t="s">
         <v>1</v>
       </c>
@@ -9632,6 +9667,9 @@
       <c r="B76">
         <v>318906</v>
       </c>
+      <c r="C76" t="s">
+        <v>406</v>
+      </c>
       <c r="D76" t="s">
         <v>1</v>
       </c>
@@ -9664,6 +9702,9 @@
       <c r="B77" t="s">
         <v>658</v>
       </c>
+      <c r="C77" t="s">
+        <v>406</v>
+      </c>
       <c r="D77" t="s">
         <v>220</v>
       </c>
@@ -9696,6 +9737,9 @@
       <c r="B78" t="s">
         <v>661</v>
       </c>
+      <c r="C78" t="s">
+        <v>406</v>
+      </c>
       <c r="D78" t="s">
         <v>220</v>
       </c>
@@ -9728,6 +9772,9 @@
       <c r="B79" t="s">
         <v>667</v>
       </c>
+      <c r="C79" t="s">
+        <v>406</v>
+      </c>
       <c r="D79" t="s">
         <v>220</v>
       </c>
@@ -9760,6 +9807,9 @@
       <c r="B80" t="s">
         <v>672</v>
       </c>
+      <c r="C80" t="s">
+        <v>406</v>
+      </c>
       <c r="D80" t="s">
         <v>220</v>
       </c>
@@ -9792,6 +9842,9 @@
       <c r="B81">
         <v>310090</v>
       </c>
+      <c r="C81" t="s">
+        <v>406</v>
+      </c>
       <c r="D81" t="s">
         <v>1</v>
       </c>
@@ -9824,6 +9877,9 @@
       <c r="B82">
         <v>310286</v>
       </c>
+      <c r="C82" t="s">
+        <v>406</v>
+      </c>
       <c r="D82" t="s">
         <v>1</v>
       </c>
@@ -9856,6 +9912,9 @@
       <c r="B83">
         <v>311975</v>
       </c>
+      <c r="C83" t="s">
+        <v>406</v>
+      </c>
       <c r="D83" t="s">
         <v>1</v>
       </c>
@@ -9891,6 +9950,9 @@
       <c r="B84">
         <v>312740</v>
       </c>
+      <c r="C84" t="s">
+        <v>406</v>
+      </c>
       <c r="D84" t="s">
         <v>1</v>
       </c>
@@ -9923,6 +9985,9 @@
       <c r="B85">
         <v>314675</v>
       </c>
+      <c r="C85" t="s">
+        <v>406</v>
+      </c>
       <c r="D85" t="s">
         <v>1</v>
       </c>
@@ -9955,6 +10020,9 @@
       <c r="B86">
         <v>314970</v>
       </c>
+      <c r="C86" t="s">
+        <v>406</v>
+      </c>
       <c r="D86" t="s">
         <v>1</v>
       </c>
@@ -9987,6 +10055,9 @@
       <c r="B87">
         <v>315743</v>
       </c>
+      <c r="C87" t="s">
+        <v>406</v>
+      </c>
       <c r="D87" t="s">
         <v>1</v>
       </c>
@@ -10022,6 +10093,9 @@
       <c r="B88">
         <v>315771</v>
       </c>
+      <c r="C88" t="s">
+        <v>406</v>
+      </c>
       <c r="D88" t="s">
         <v>1</v>
       </c>
@@ -10057,6 +10131,9 @@
       <c r="B89">
         <v>315890</v>
       </c>
+      <c r="C89" t="s">
+        <v>406</v>
+      </c>
       <c r="D89" t="s">
         <v>1</v>
       </c>
@@ -10092,6 +10169,9 @@
       <c r="B90">
         <v>315945</v>
       </c>
+      <c r="C90" t="s">
+        <v>406</v>
+      </c>
       <c r="D90" t="s">
         <v>1</v>
       </c>
@@ -10127,6 +10207,9 @@
       <c r="B91">
         <v>316256</v>
       </c>
+      <c r="C91" t="s">
+        <v>406</v>
+      </c>
       <c r="D91" t="s">
         <v>1</v>
       </c>
@@ -10159,6 +10242,9 @@
       <c r="B92">
         <v>316686</v>
       </c>
+      <c r="C92" t="s">
+        <v>406</v>
+      </c>
       <c r="D92" t="s">
         <v>1</v>
       </c>
@@ -10191,6 +10277,9 @@
       <c r="B93">
         <v>317508</v>
       </c>
+      <c r="C93" t="s">
+        <v>406</v>
+      </c>
       <c r="D93" t="s">
         <v>1</v>
       </c>
@@ -10223,6 +10312,9 @@
       <c r="B94">
         <v>317615</v>
       </c>
+      <c r="C94" t="s">
+        <v>406</v>
+      </c>
       <c r="D94" t="s">
         <v>1</v>
       </c>
@@ -10258,6 +10350,9 @@
       <c r="B95">
         <v>317618</v>
       </c>
+      <c r="C95" t="s">
+        <v>406</v>
+      </c>
       <c r="D95" t="s">
         <v>1</v>
       </c>
@@ -10290,6 +10385,9 @@
       <c r="B96">
         <v>318292</v>
       </c>
+      <c r="C96" t="s">
+        <v>406</v>
+      </c>
       <c r="D96" t="s">
         <v>1</v>
       </c>
@@ -10322,6 +10420,9 @@
       <c r="B97">
         <v>318778</v>
       </c>
+      <c r="C97" t="s">
+        <v>406</v>
+      </c>
       <c r="D97" t="s">
         <v>1</v>
       </c>
@@ -10354,6 +10455,9 @@
       <c r="B98">
         <v>319555</v>
       </c>
+      <c r="C98" t="s">
+        <v>406</v>
+      </c>
       <c r="D98" t="s">
         <v>1</v>
       </c>
@@ -10386,6 +10490,9 @@
       <c r="B99">
         <v>318964</v>
       </c>
+      <c r="C99" t="s">
+        <v>406</v>
+      </c>
       <c r="D99" t="s">
         <v>1</v>
       </c>
@@ -10418,6 +10525,9 @@
       <c r="B100">
         <v>319539</v>
       </c>
+      <c r="C100" t="s">
+        <v>406</v>
+      </c>
       <c r="D100" t="s">
         <v>1</v>
       </c>
@@ -10453,6 +10563,9 @@
       <c r="B101">
         <v>319675</v>
       </c>
+      <c r="C101" t="s">
+        <v>406</v>
+      </c>
       <c r="D101" t="s">
         <v>1</v>
       </c>
@@ -10485,6 +10598,9 @@
       <c r="B102">
         <v>311913</v>
       </c>
+      <c r="C102" t="s">
+        <v>406</v>
+      </c>
       <c r="D102" t="s">
         <v>1</v>
       </c>
@@ -10517,6 +10633,9 @@
       <c r="B103">
         <v>313784</v>
       </c>
+      <c r="C103" t="s">
+        <v>406</v>
+      </c>
       <c r="D103" t="s">
         <v>1</v>
       </c>
@@ -10549,6 +10668,9 @@
       <c r="B104">
         <v>314464</v>
       </c>
+      <c r="C104" t="s">
+        <v>406</v>
+      </c>
       <c r="D104" t="s">
         <v>1</v>
       </c>
@@ -10581,6 +10703,9 @@
       <c r="B105">
         <v>314860</v>
       </c>
+      <c r="C105" t="s">
+        <v>406</v>
+      </c>
       <c r="D105" t="s">
         <v>1</v>
       </c>
@@ -10613,6 +10738,9 @@
       <c r="B106">
         <v>315116</v>
       </c>
+      <c r="C106" t="s">
+        <v>406</v>
+      </c>
       <c r="D106" t="s">
         <v>1</v>
       </c>
@@ -10645,6 +10773,9 @@
       <c r="B107">
         <v>315175</v>
       </c>
+      <c r="C107" t="s">
+        <v>406</v>
+      </c>
       <c r="D107" t="s">
         <v>1</v>
       </c>
@@ -10677,6 +10808,9 @@
       <c r="B108">
         <v>315177</v>
       </c>
+      <c r="C108" t="s">
+        <v>406</v>
+      </c>
       <c r="D108" t="s">
         <v>1</v>
       </c>
@@ -10709,6 +10843,9 @@
       <c r="B109">
         <v>315182</v>
       </c>
+      <c r="C109" t="s">
+        <v>406</v>
+      </c>
       <c r="D109" t="s">
         <v>1</v>
       </c>
@@ -10741,6 +10878,9 @@
       <c r="B110">
         <v>317813</v>
       </c>
+      <c r="C110" t="s">
+        <v>406</v>
+      </c>
       <c r="D110" t="s">
         <v>1</v>
       </c>
@@ -10773,6 +10913,9 @@
       <c r="B111" t="s">
         <v>769</v>
       </c>
+      <c r="C111" t="s">
+        <v>406</v>
+      </c>
       <c r="D111" t="s">
         <v>220</v>
       </c>
@@ -10805,6 +10948,9 @@
       <c r="B112" t="s">
         <v>774</v>
       </c>
+      <c r="C112" t="s">
+        <v>406</v>
+      </c>
       <c r="D112" t="s">
         <v>220</v>
       </c>
@@ -10837,6 +10983,9 @@
       <c r="B113" t="s">
         <v>777</v>
       </c>
+      <c r="C113" t="s">
+        <v>406</v>
+      </c>
       <c r="D113" t="s">
         <v>220</v>
       </c>
@@ -10869,6 +11018,9 @@
       <c r="B114" t="s">
         <v>781</v>
       </c>
+      <c r="C114" t="s">
+        <v>406</v>
+      </c>
       <c r="D114" t="s">
         <v>220</v>
       </c>
@@ -10901,6 +11053,9 @@
       <c r="B115" t="s">
         <v>787</v>
       </c>
+      <c r="C115" t="s">
+        <v>406</v>
+      </c>
       <c r="D115" t="s">
         <v>220</v>
       </c>
@@ -10933,6 +11088,9 @@
       <c r="B116">
         <v>312238</v>
       </c>
+      <c r="C116" t="s">
+        <v>406</v>
+      </c>
       <c r="D116" t="s">
         <v>1</v>
       </c>
@@ -10965,6 +11123,9 @@
       <c r="B117">
         <v>312631</v>
       </c>
+      <c r="C117" t="s">
+        <v>406</v>
+      </c>
       <c r="D117" t="s">
         <v>1</v>
       </c>
@@ -10997,6 +11158,9 @@
       <c r="B118">
         <v>313969</v>
       </c>
+      <c r="C118" t="s">
+        <v>406</v>
+      </c>
       <c r="D118" t="s">
         <v>1</v>
       </c>
@@ -11032,6 +11196,9 @@
       <c r="B119">
         <v>313971</v>
       </c>
+      <c r="C119" t="s">
+        <v>406</v>
+      </c>
       <c r="D119" t="s">
         <v>1</v>
       </c>
@@ -11064,6 +11231,9 @@
       <c r="B120">
         <v>314962</v>
       </c>
+      <c r="C120" t="s">
+        <v>406</v>
+      </c>
       <c r="D120" t="s">
         <v>1</v>
       </c>
@@ -11096,6 +11266,9 @@
       <c r="B121">
         <v>317202</v>
       </c>
+      <c r="C121" t="s">
+        <v>406</v>
+      </c>
       <c r="D121" t="s">
         <v>1</v>
       </c>
@@ -11128,6 +11301,9 @@
       <c r="B122">
         <v>317319</v>
       </c>
+      <c r="C122" t="s">
+        <v>406</v>
+      </c>
       <c r="D122" t="s">
         <v>1</v>
       </c>
@@ -11160,6 +11336,9 @@
       <c r="B123">
         <v>318196</v>
       </c>
+      <c r="C123" t="s">
+        <v>406</v>
+      </c>
       <c r="D123" t="s">
         <v>1</v>
       </c>
@@ -11192,6 +11371,9 @@
       <c r="B124">
         <v>319440</v>
       </c>
+      <c r="C124" t="s">
+        <v>406</v>
+      </c>
       <c r="D124" t="s">
         <v>1</v>
       </c>
@@ -11224,6 +11406,9 @@
       <c r="B125">
         <v>319704</v>
       </c>
+      <c r="C125" t="s">
+        <v>406</v>
+      </c>
       <c r="D125" t="s">
         <v>1</v>
       </c>
@@ -11256,6 +11441,9 @@
       <c r="B126">
         <v>310356</v>
       </c>
+      <c r="C126" t="s">
+        <v>406</v>
+      </c>
       <c r="D126" t="s">
         <v>1</v>
       </c>
@@ -11288,6 +11476,9 @@
       <c r="B127">
         <v>310375</v>
       </c>
+      <c r="C127" t="s">
+        <v>406</v>
+      </c>
       <c r="D127" t="s">
         <v>1</v>
       </c>
@@ -11320,6 +11511,9 @@
       <c r="B128">
         <v>310576</v>
       </c>
+      <c r="C128" t="s">
+        <v>406</v>
+      </c>
       <c r="D128" t="s">
         <v>1</v>
       </c>
@@ -11352,6 +11546,9 @@
       <c r="B129">
         <v>310674</v>
       </c>
+      <c r="C129" t="s">
+        <v>406</v>
+      </c>
       <c r="D129" t="s">
         <v>1</v>
       </c>
@@ -11384,6 +11581,9 @@
       <c r="B130">
         <v>311458</v>
       </c>
+      <c r="C130" t="s">
+        <v>406</v>
+      </c>
       <c r="D130" t="s">
         <v>1</v>
       </c>
@@ -11416,6 +11616,9 @@
       <c r="B131">
         <v>311606</v>
       </c>
+      <c r="C131" t="s">
+        <v>406</v>
+      </c>
       <c r="D131" t="s">
         <v>1</v>
       </c>
@@ -11448,6 +11651,9 @@
       <c r="B132">
         <v>312940</v>
       </c>
+      <c r="C132" t="s">
+        <v>406</v>
+      </c>
       <c r="D132" t="s">
         <v>1</v>
       </c>
@@ -11480,6 +11686,9 @@
       <c r="B133">
         <v>313336</v>
       </c>
+      <c r="C133" t="s">
+        <v>406</v>
+      </c>
       <c r="D133" t="s">
         <v>1</v>
       </c>
@@ -11512,6 +11721,9 @@
       <c r="B134">
         <v>313638</v>
       </c>
+      <c r="C134" t="s">
+        <v>406</v>
+      </c>
       <c r="D134" t="s">
         <v>1</v>
       </c>
@@ -11547,6 +11759,9 @@
       <c r="B135">
         <v>315123</v>
       </c>
+      <c r="C135" t="s">
+        <v>406</v>
+      </c>
       <c r="D135" t="s">
         <v>1</v>
       </c>
@@ -11582,6 +11797,9 @@
       <c r="B136">
         <v>315830</v>
       </c>
+      <c r="C136" t="s">
+        <v>406</v>
+      </c>
       <c r="D136" t="s">
         <v>1</v>
       </c>
@@ -11614,6 +11832,9 @@
       <c r="B137">
         <v>316349</v>
       </c>
+      <c r="C137" t="s">
+        <v>406</v>
+      </c>
       <c r="D137" t="s">
         <v>1</v>
       </c>
@@ -11646,6 +11867,9 @@
       <c r="B138">
         <v>316510</v>
       </c>
+      <c r="C138" t="s">
+        <v>406</v>
+      </c>
       <c r="D138" t="s">
         <v>1</v>
       </c>
@@ -11678,6 +11902,9 @@
       <c r="B139">
         <v>317400</v>
       </c>
+      <c r="C139" t="s">
+        <v>406</v>
+      </c>
       <c r="D139" t="s">
         <v>1</v>
       </c>
@@ -11710,6 +11937,9 @@
       <c r="B140">
         <v>318450</v>
       </c>
+      <c r="C140" t="s">
+        <v>406</v>
+      </c>
       <c r="D140" t="s">
         <v>1</v>
       </c>
@@ -11742,6 +11972,9 @@
       <c r="B141">
         <v>318500</v>
       </c>
+      <c r="C141" t="s">
+        <v>406</v>
+      </c>
       <c r="D141" t="s">
         <v>1</v>
       </c>
@@ -11777,6 +12010,9 @@
       <c r="B142">
         <v>319100</v>
       </c>
+      <c r="C142" t="s">
+        <v>406</v>
+      </c>
       <c r="D142" t="s">
         <v>1</v>
       </c>
@@ -11812,6 +12048,9 @@
       <c r="B143" t="s">
         <v>873</v>
       </c>
+      <c r="C143" t="s">
+        <v>406</v>
+      </c>
       <c r="D143" t="s">
         <v>220</v>
       </c>
@@ -11844,6 +12083,9 @@
       <c r="B144" t="s">
         <v>876</v>
       </c>
+      <c r="C144" t="s">
+        <v>406</v>
+      </c>
       <c r="D144" t="s">
         <v>220</v>
       </c>
@@ -11876,6 +12118,9 @@
       <c r="B145" t="s">
         <v>879</v>
       </c>
+      <c r="C145" t="s">
+        <v>406</v>
+      </c>
       <c r="D145" t="s">
         <v>220</v>
       </c>
@@ -11908,6 +12153,9 @@
       <c r="B146" t="s">
         <v>882</v>
       </c>
+      <c r="C146" t="s">
+        <v>406</v>
+      </c>
       <c r="D146" t="s">
         <v>220</v>
       </c>
@@ -11940,6 +12188,9 @@
       <c r="B147">
         <v>311949</v>
       </c>
+      <c r="C147" t="s">
+        <v>406</v>
+      </c>
       <c r="D147" t="s">
         <v>1</v>
       </c>
@@ -11972,6 +12223,9 @@
       <c r="B148">
         <v>312635</v>
       </c>
+      <c r="C148" t="s">
+        <v>406</v>
+      </c>
       <c r="D148" t="s">
         <v>1</v>
       </c>
@@ -12007,6 +12261,9 @@
       <c r="B149">
         <v>312719</v>
       </c>
+      <c r="C149" t="s">
+        <v>406</v>
+      </c>
       <c r="D149" t="s">
         <v>1</v>
       </c>
@@ -12039,6 +12296,9 @@
       <c r="B150">
         <v>312724</v>
       </c>
+      <c r="C150" t="s">
+        <v>406</v>
+      </c>
       <c r="D150" t="s">
         <v>1</v>
       </c>
@@ -12071,6 +12331,9 @@
       <c r="B151">
         <v>314456</v>
       </c>
+      <c r="C151" t="s">
+        <v>406</v>
+      </c>
       <c r="D151" t="s">
         <v>1</v>
       </c>
@@ -12103,6 +12366,9 @@
       <c r="B152">
         <v>315303</v>
       </c>
+      <c r="C152" t="s">
+        <v>406</v>
+      </c>
       <c r="D152" t="s">
         <v>1</v>
       </c>
@@ -12135,6 +12401,9 @@
       <c r="B153">
         <v>315996</v>
       </c>
+      <c r="C153" t="s">
+        <v>406</v>
+      </c>
       <c r="D153" t="s">
         <v>1</v>
       </c>
@@ -12166,6 +12435,9 @@
       </c>
       <c r="B154">
         <v>316853</v>
+      </c>
+      <c r="C154" t="s">
+        <v>406</v>
       </c>
       <c r="D154" t="s">
         <v>1</v>

</xml_diff>